<commit_message>
#Please enter the commit message for your changes. Lines starting  Export Functionality
</commit_message>
<xml_diff>
--- a/Srini_ApplicationStatus_21_2_20.xlsx
+++ b/Srini_ApplicationStatus_21_2_20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erupa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E60DD9-2406-40D1-A450-F6157417E5A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0F809A-921F-4C95-817B-25BB70193E04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{5F337796-13E9-46E3-830E-646228CEE590}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="280">
   <si>
     <t>Customer Master</t>
   </si>
@@ -1655,7 +1655,7 @@
   <dimension ref="C2:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2999,12 +2999,15 @@
         <v>276</v>
       </c>
     </row>
-    <row r="113" spans="5:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="5:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E113" s="22" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F113" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="114" spans="5:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E114" t="s">
         <v>278</v>
       </c>

</xml_diff>

<commit_message>
Overdue Based on Category
</commit_message>
<xml_diff>
--- a/Srini_ApplicationStatus_21_2_20.xlsx
+++ b/Srini_ApplicationStatus_21_2_20.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="299">
   <si>
     <t>Customer Master</t>
   </si>
@@ -1052,6 +1052,12 @@
   </si>
   <si>
     <t>Dashboard- Hover Over Overdue</t>
+  </si>
+  <si>
+    <t>(RID, Family, S.No, Overdue Age, Overall the overdue)</t>
+  </si>
+  <si>
+    <t>Master - Overdue for individual Product Category</t>
   </si>
 </sst>
 </file>
@@ -1702,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H133"/>
+  <dimension ref="C2:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G133" sqref="G133"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,7 +1719,7 @@
     <col min="3" max="3" width="8.7109375" style="1"/>
     <col min="4" max="4" width="47.7109375" customWidth="1"/>
     <col min="5" max="5" width="33.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3114,6 +3120,9 @@
       <c r="E123" t="s">
         <v>285</v>
       </c>
+      <c r="G123" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="124" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E124" t="s">
@@ -3142,6 +3151,9 @@
       <c r="E128" t="s">
         <v>289</v>
       </c>
+      <c r="G128" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="129" spans="5:7" ht="30" x14ac:dyDescent="0.25">
       <c r="E129" s="22" t="s">
@@ -3166,11 +3178,19 @@
         <v>294</v>
       </c>
     </row>
-    <row r="133" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:7" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E133" t="s">
         <v>296</v>
       </c>
-      <c r="G133" t="s">
+      <c r="F133" s="22" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="134" spans="5:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E134" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="G134" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3317,8 +3337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:L10"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Repair Report Query Update
</commit_message>
<xml_diff>
--- a/Srini_ApplicationStatus_21_2_20.xlsx
+++ b/Srini_ApplicationStatus_21_2_20.xlsx
@@ -1755,8 +1755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Repair Report Query Updates
</commit_message>
<xml_diff>
--- a/Srini_ApplicationStatus_21_2_20.xlsx
+++ b/Srini_ApplicationStatus_21_2_20.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,15 +27,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$C$2:$G$105</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1755,8 +1750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>